<commit_message>
Perfected the generate email function.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -481,12 +477,14 @@
           <t>Abwoga, Adrian Jared Paul</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>36694</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2000-06-17</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>abwoga,.adrianeogch@gmail.com</t>
+          <t>A.Adrian@gmail.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -507,12 +505,14 @@
           <t>Akong'o, Shanelle Hilda Anyango</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>37209</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2001-11-14</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>akong'o,.shanellejrzzz@gmail.com</t>
+          <t>A.Shanelle@gmail.com</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -533,12 +533,14 @@
           <t>Ang'edu, Jude Ocomil</t>
         </is>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>37854</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2003-08-21</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ang'edu,.judeskrxi@gmail.com</t>
+          <t>A.Jude@gmail.com</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -559,12 +561,14 @@
           <t>Arunga, Kyla Neema</t>
         </is>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>37920</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2003-10-26</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>arunga,.kylafytld@gmail.com</t>
+          <t>A.Kyla@gmail.com</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -585,12 +589,14 @@
           <t>Atenya, Anthony Magunga Ikobwa</t>
         </is>
       </c>
-      <c r="D6" s="2" t="n">
-        <v>37332</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2002-03-17</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>atenya,.anthonybsfhe@gmail.com</t>
+          <t>A.Anthony@gmail.com</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -611,12 +617,14 @@
           <t>Budembeshe, Moses Kasuni</t>
         </is>
       </c>
-      <c r="D7" s="2" t="n">
-        <v>37311</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2002-02-24</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>budembeshe,.mosespkadk@gmail.com</t>
+          <t>B.Moses@gmail.com</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -637,12 +645,14 @@
           <t>Dessalegn, Kalid Geleta</t>
         </is>
       </c>
-      <c r="D8" s="2" t="n">
-        <v>36776</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2000-09-07</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>dessalegn,.kalidxigka@gmail.com</t>
+          <t>D.Kalid@gmail.com</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -663,12 +673,14 @@
           <t>Epetet, Keith Lokwei</t>
         </is>
       </c>
-      <c r="D9" s="2" t="n">
-        <v>37050</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2001-06-08</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>epetet,.keithcrwcf@gmail.com</t>
+          <t>E.Keith@gmail.com</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -689,12 +701,14 @@
           <t>Ger, David Otieno</t>
         </is>
       </c>
-      <c r="D10" s="2" t="n">
-        <v>36919</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2001-01-28</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ger,.davidgkcex@gmail.com</t>
+          <t>G.David@gmail.com</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -715,12 +729,14 @@
           <t>Githinji, Don Moses Thigiti</t>
         </is>
       </c>
-      <c r="D11" s="2" t="n">
-        <v>36628</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2000-04-12</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>githinji,.donfvnsa@gmail.com</t>
+          <t>G.Don@gmail.com</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -741,12 +757,14 @@
           <t>Haji, Ashir Ali</t>
         </is>
       </c>
-      <c r="D12" s="2" t="n">
-        <v>37785</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2003-06-13</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>haji,.ashirxxihf@gmail.com</t>
+          <t>H.Ashir@gmail.com</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -767,12 +785,14 @@
           <t>Hassan, Fardowsa Abduhakim</t>
         </is>
       </c>
-      <c r="D13" s="2" t="n">
-        <v>36789</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2000-09-20</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>hassan,.fardowsaeemam@gmail.com</t>
+          <t>H.Fardowsa@gmail.com</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -793,12 +813,14 @@
           <t>Ismail, Ruweida Ali</t>
         </is>
       </c>
-      <c r="D14" s="2" t="n">
-        <v>36624</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2000-04-08</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ismail,.ruweidamhedv@gmail.com</t>
+          <t>I.Ruweida@gmail.com</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -819,12 +841,14 @@
           <t>Johnson, Myles Adebayo</t>
         </is>
       </c>
-      <c r="D15" s="2" t="n">
-        <v>37008</v>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2001-04-27</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>johnson,.mylescwiun@gmail.com</t>
+          <t>J.Myles@gmail.com</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -845,12 +869,14 @@
           <t>Kamau, Ann Mumbi</t>
         </is>
       </c>
-      <c r="D16" s="2" t="n">
-        <v>37223</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2001-11-28</t>
+        </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>kamau,.annbybzi@gmail.com</t>
+          <t>K.Ann@gmail.com</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -871,12 +897,14 @@
           <t>Kangethe, Sharon Wanjiru</t>
         </is>
       </c>
-      <c r="D17" s="2" t="n">
-        <v>36576</v>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2000-02-20</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>kangethe,.sharonkvufw@gmail.com</t>
+          <t>K.Sharon@gmail.com</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -897,12 +925,14 @@
           <t>Karanu, Neema Muthoni</t>
         </is>
       </c>
-      <c r="D18" s="2" t="n">
-        <v>37219</v>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2001-11-24</t>
+        </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>karanu,.neemauauez@gmail.com</t>
+          <t>K.Neema@gmail.com</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -923,12 +953,14 @@
           <t>Kiarie, Samuel Ndungu</t>
         </is>
       </c>
-      <c r="D19" s="2" t="n">
-        <v>36686</v>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2000-06-09</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>kiarie,.samuelatrtu@gmail.com</t>
+          <t>K.Samuel@gmail.com</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -949,12 +981,14 @@
           <t>Kihara, Shannon Kendi</t>
         </is>
       </c>
-      <c r="D20" s="2" t="n">
-        <v>37543</v>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2002-10-14</t>
+        </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>kihara,.shannonzyqwg@gmail.com</t>
+          <t>K.Shannon@gmail.com</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -975,12 +1009,14 @@
           <t>Kimutai, Peter Kibet</t>
         </is>
       </c>
-      <c r="D21" s="2" t="n">
-        <v>37515</v>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2002-09-16</t>
+        </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>kimutai,.peterabwqu@gmail.com</t>
+          <t>K.Peter@gmail.com</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1001,12 +1037,14 @@
           <t>Kinyua, Victor Mfana</t>
         </is>
       </c>
-      <c r="D22" s="2" t="n">
-        <v>37922</v>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2003-10-28</t>
+        </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>kinyua,.victoriipdx@gmail.com</t>
+          <t>K.Victor@gmail.com</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1027,12 +1065,14 @@
           <t>Kirema, Ian Muteithia</t>
         </is>
       </c>
-      <c r="D23" s="2" t="n">
-        <v>36951</v>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2001-03-01</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>kirema,.ianrnsdw@gmail.com</t>
+          <t>K.Ian@gmail.com</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1053,12 +1093,14 @@
           <t>Kithae, Eric Muriithi</t>
         </is>
       </c>
-      <c r="D24" s="2" t="n">
-        <v>36801</v>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2000-10-02</t>
+        </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>kithae,.ericaxjvk@gmail.com</t>
+          <t>K.Eric@gmail.com</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1079,12 +1121,14 @@
           <t>Korir, Kevin Kimutai</t>
         </is>
       </c>
-      <c r="D25" s="2" t="n">
-        <v>37555</v>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2002-10-26</t>
+        </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>korir,.kevintgadb@gmail.com</t>
+          <t>K.Kevin@gmail.com</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1105,12 +1149,14 @@
           <t>Kwoba, Alex Wafula</t>
         </is>
       </c>
-      <c r="D26" s="2" t="n">
-        <v>37372</v>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2002-04-26</t>
+        </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>kwoba,.alexkqfry@gmail.com</t>
+          <t>K.Alex@gmail.com</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1131,12 +1177,14 @@
           <t>Maritim, Kelvin Kipngeno</t>
         </is>
       </c>
-      <c r="D27" s="2" t="n">
-        <v>36822</v>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2000-10-23</t>
+        </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>maritim,.kelvinvhfzq@gmail.com</t>
+          <t>M.Kelvin@gmail.com</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1157,12 +1205,14 @@
           <t>Masaka, Zivai Takadiwa David</t>
         </is>
       </c>
-      <c r="D28" s="2" t="n">
-        <v>37443</v>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2002-07-06</t>
+        </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>masaka,.zivaidaavj@gmail.com</t>
+          <t>M.Zivai@gmail.com</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1183,12 +1233,14 @@
           <t>Mohamed, Ally Mahamud</t>
         </is>
       </c>
-      <c r="D29" s="2" t="n">
-        <v>37715</v>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2003-04-04</t>
+        </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>mohamed,.allysgygt@gmail.com</t>
+          <t>M.Ally@gmail.com</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1209,12 +1261,14 @@
           <t>Morekwa, David Nyamongo</t>
         </is>
       </c>
-      <c r="D30" s="2" t="n">
-        <v>36935</v>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2001-02-13</t>
+        </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>morekwa,.davidpghlv@gmail.com</t>
+          <t>M.David@gmail.com</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1235,12 +1289,14 @@
           <t>Mugambi, Kelvin Karani</t>
         </is>
       </c>
-      <c r="D31" s="2" t="n">
-        <v>36626</v>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2000-04-10</t>
+        </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>mugambi,.kelvindxjln@gmail.com</t>
+          <t>M.Kelvin@gmail.com</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1261,12 +1317,14 @@
           <t>Muhia, Victor Mwaura</t>
         </is>
       </c>
-      <c r="D32" s="2" t="n">
-        <v>36795</v>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2000-09-26</t>
+        </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>muhia,.victorqwlsn@gmail.com</t>
+          <t>M.Victor@gmail.com</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1287,12 +1345,14 @@
           <t>Muiyuro, Natasha Waithira</t>
         </is>
       </c>
-      <c r="D33" s="2" t="n">
-        <v>37487</v>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2002-08-19</t>
+        </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>muiyuro,.natashaufbpg@gmail.com</t>
+          <t>M.Natasha@gmail.com</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1313,12 +1373,14 @@
           <t>Muli, Grace Kanini</t>
         </is>
       </c>
-      <c r="D34" s="2" t="n">
-        <v>36643</v>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2000-04-27</t>
+        </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>muli,.graceosuvo@gmail.com</t>
+          <t>M.Grace@gmail.com</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1339,12 +1401,14 @@
           <t>Muroki, Mark Gichuhi</t>
         </is>
       </c>
-      <c r="D35" s="2" t="n">
-        <v>37253</v>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2001-12-28</t>
+        </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>muroki,.markupnyq@gmail.com</t>
+          <t>M.Mark@gmail.com</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1365,12 +1429,14 @@
           <t>Mutaki, Ruby Mbete</t>
         </is>
       </c>
-      <c r="D36" s="2" t="n">
-        <v>37424</v>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2002-06-17</t>
+        </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>mutaki,.rubyukriu@gmail.com</t>
+          <t>M.Ruby@gmail.com</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1391,12 +1457,14 @@
           <t>Mutua, Franklin Karanja</t>
         </is>
       </c>
-      <c r="D37" s="2" t="n">
-        <v>37915</v>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2003-10-21</t>
+        </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>mutua,.franklinrjekk@gmail.com</t>
+          <t>M.Franklin@gmail.com</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1417,12 +1485,14 @@
           <t>Mutunga, Eric Kiamba</t>
         </is>
       </c>
-      <c r="D38" s="2" t="n">
-        <v>37813</v>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2003-07-11</t>
+        </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>mutunga,.ericnvyld@gmail.com</t>
+          <t>M.Eric@gmail.com</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1443,12 +1513,14 @@
           <t>Mutunga, Patience Kamanthe</t>
         </is>
       </c>
-      <c r="D39" s="2" t="n">
-        <v>36746</v>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2000-08-08</t>
+        </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>mutunga,.patiencepactl@gmail.com</t>
+          <t>M.Patience@gmail.com</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1469,12 +1541,14 @@
           <t>Mwanda, George Josiah</t>
         </is>
       </c>
-      <c r="D40" s="2" t="n">
-        <v>36576</v>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2000-02-20</t>
+        </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>mwanda,.georgelgfar@gmail.com</t>
+          <t>M.George@gmail.com</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1495,12 +1569,14 @@
           <t>Nabaala, Andrew Kasaine</t>
         </is>
       </c>
-      <c r="D41" s="2" t="n">
-        <v>37099</v>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2001-07-27</t>
+        </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>nabaala,.andrewzsmvq@gmail.com</t>
+          <t>N.Andrew@gmail.com</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1521,12 +1597,14 @@
           <t>Naibei, Monicah</t>
         </is>
       </c>
-      <c r="D42" s="2" t="n">
-        <v>37588</v>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2002-11-28</t>
+        </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>naibei,.monicaheeuqj@gmail.com</t>
+          <t>N.Monicah@gmail.com</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1547,12 +1625,14 @@
           <t>Ndambiri, Yvonne Nyambura</t>
         </is>
       </c>
-      <c r="D43" s="2" t="n">
-        <v>37458</v>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2002-07-21</t>
+        </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ndambiri,.yvonnelotbq@gmail.com</t>
+          <t>N.Yvonne@gmail.com</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1573,12 +1653,14 @@
           <t>Ndungu, Sarah Laura Wangari</t>
         </is>
       </c>
-      <c r="D44" s="2" t="n">
-        <v>37895</v>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2003-10-01</t>
+        </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ndungu,.sarahlvjnp@gmail.com</t>
+          <t>N.Sarah@gmail.com</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1599,12 +1681,14 @@
           <t>Ng'ang'a, Ian Mutuge</t>
         </is>
       </c>
-      <c r="D45" s="2" t="n">
-        <v>36914</v>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2001-01-23</t>
+        </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ng'ang'a,.ianqbhgm@gmail.com</t>
+          <t>N.Ian@gmail.com</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1625,12 +1709,14 @@
           <t>Ngeno, Alvin Kipkurui</t>
         </is>
       </c>
-      <c r="D46" s="2" t="n">
-        <v>37612</v>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2002-12-22</t>
+        </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ngeno,.alvinetfhp@gmail.com</t>
+          <t>N.Alvin@gmail.com</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1651,12 +1737,14 @@
           <t>Ngigi, Michael Macharia</t>
         </is>
       </c>
-      <c r="D47" s="2" t="n">
-        <v>37844</v>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2003-08-11</t>
+        </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>ngigi,.michaelgxudt@gmail.com</t>
+          <t>N.Michael@gmail.com</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1677,12 +1765,14 @@
           <t>Njuguna, Elizabeth Njoki</t>
         </is>
       </c>
-      <c r="D48" s="2" t="n">
-        <v>36714</v>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2000-07-07</t>
+        </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>njuguna,.elizabethccyex@gmail.com</t>
+          <t>N.Elizabeth@gmail.com</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1703,12 +1793,14 @@
           <t>Nugi, Andrew Kiarie</t>
         </is>
       </c>
-      <c r="D49" s="2" t="n">
-        <v>37726</v>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2003-04-15</t>
+        </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>nugi,.andrewcbvex@gmail.com</t>
+          <t>N.Andrew@gmail.com</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1729,12 +1821,14 @@
           <t>Nyambura, Erica</t>
         </is>
       </c>
-      <c r="D50" s="2" t="n">
-        <v>37494</v>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2002-08-26</t>
+        </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>nyambura,.ericaxykoo@gmail.com</t>
+          <t>N.Erica@gmail.com</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -1755,12 +1849,14 @@
           <t>Nzioki, Maureen Mutete</t>
         </is>
       </c>
-      <c r="D51" s="2" t="n">
-        <v>37534</v>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2002-10-05</t>
+        </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>nzioki,.maureenjxhhi@gmail.com</t>
+          <t>N.Maureen@gmail.com</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -1781,12 +1877,14 @@
           <t>Ochanda, Steven Joel Jona</t>
         </is>
       </c>
-      <c r="D52" s="2" t="n">
-        <v>36618</v>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2000-04-02</t>
+        </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>ochanda,.stevenedzgg@gmail.com</t>
+          <t>O.Steven@gmail.com</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -1807,12 +1905,14 @@
           <t>Ogutu, Brenda Mary Anyango</t>
         </is>
       </c>
-      <c r="D53" s="2" t="n">
-        <v>37370</v>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2002-04-24</t>
+        </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>ogutu,.brendavcyks@gmail.com</t>
+          <t>O.Brenda@gmail.com</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -1833,12 +1933,14 @@
           <t>Ombeni, Mwenzangu Faraja</t>
         </is>
       </c>
-      <c r="D54" s="2" t="n">
-        <v>37228</v>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2001-12-03</t>
+        </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>ombeni,.mwenzanguuxqtu@gmail.com</t>
+          <t>O.Mwenzangu@gmail.com</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -1859,12 +1961,14 @@
           <t>Ombongi, Caleb Magare</t>
         </is>
       </c>
-      <c r="D55" s="2" t="n">
-        <v>37526</v>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2002-09-27</t>
+        </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>ombongi,.calebniaxd@gmail.com</t>
+          <t>O.Caleb@gmail.com</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -1885,12 +1989,14 @@
           <t>Orony, Charis Ng'wono</t>
         </is>
       </c>
-      <c r="D56" s="2" t="n">
-        <v>36541</v>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2000-01-16</t>
+        </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>orony,.charisedsbk@gmail.com</t>
+          <t>O.Charis@gmail.com</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -1911,12 +2017,14 @@
           <t>Owens, Nicole Owens</t>
         </is>
       </c>
-      <c r="D57" s="2" t="n">
-        <v>36783</v>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2000-09-14</t>
+        </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>owens,.nicoleikmxb@gmail.com</t>
+          <t>O.Nicole@gmail.com</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -1937,12 +2045,14 @@
           <t>Patel, Jay Hirji</t>
         </is>
       </c>
-      <c r="D58" s="2" t="n">
-        <v>37797</v>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2003-06-25</t>
+        </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>patel,.jaybywqe@gmail.com</t>
+          <t>P.Jay@gmail.com</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -1963,12 +2073,14 @@
           <t>Tonui, Martin</t>
         </is>
       </c>
-      <c r="D59" s="2" t="n">
-        <v>37409</v>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2002-06-02</t>
+        </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>tonui,.martincbxnp@gmail.com</t>
+          <t>T.Martin@gmail.com</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -1989,12 +2101,14 @@
           <t>Tum, Bramwel Kipchirchir</t>
         </is>
       </c>
-      <c r="D60" s="2" t="n">
-        <v>36928</v>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2001-02-06</t>
+        </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>tum,.bramwelbygfq@gmail.com</t>
+          <t>T.Bramwel@gmail.com</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2015,12 +2129,14 @@
           <t>Wachira, Joy Muthoni</t>
         </is>
       </c>
-      <c r="D61" s="2" t="n">
-        <v>37110</v>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2001-08-07</t>
+        </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>wachira,.joynftzw@gmail.com</t>
+          <t>W.Joy@gmail.com</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2041,12 +2157,14 @@
           <t>Wakaba, Rosemary Njeri</t>
         </is>
       </c>
-      <c r="D62" s="2" t="n">
-        <v>36536</v>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2000-01-11</t>
+        </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>wakaba,.rosemaryrmhmr@gmail.com</t>
+          <t>W.Rosemary@gmail.com</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2067,12 +2185,14 @@
           <t>Wanjao, Louis Mbugua</t>
         </is>
       </c>
-      <c r="D63" s="2" t="n">
-        <v>37001</v>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2001-04-20</t>
+        </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>wanjao,.louisejvhy@gmail.com</t>
+          <t>W.Louis@gmail.com</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2093,12 +2213,14 @@
           <t>Waweru, Monika Ng'endo</t>
         </is>
       </c>
-      <c r="D64" s="2" t="n">
-        <v>37396</v>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2002-05-20</t>
+        </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>waweru,.monikaabhog@gmail.com</t>
+          <t>W.Monika@gmail.com</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2119,12 +2241,14 @@
           <t>Waweru, Trevor Kariuki</t>
         </is>
       </c>
-      <c r="D65" s="2" t="n">
-        <v>37365</v>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2002-04-19</t>
+        </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>waweru,.trevorkduxo@gmail.com</t>
+          <t>W.Trevor@gmail.com</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">

</xml_diff>

<commit_message>
Lower case first letter.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -484,7 +484,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>A.Adrian@gmail.com</t>
+          <t>a.Adrian@gmail.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>A.Shanelle@gmail.com</t>
+          <t>a.Shanelle@gmail.com</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>A.Jude@gmail.com</t>
+          <t>a.Jude@gmail.com</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>A.Kyla@gmail.com</t>
+          <t>a.Kyla@gmail.com</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>A.Anthony@gmail.com</t>
+          <t>a.Anthony@gmail.com</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>B.Moses@gmail.com</t>
+          <t>b.Moses@gmail.com</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>D.Kalid@gmail.com</t>
+          <t>d.Kalid@gmail.com</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>E.Keith@gmail.com</t>
+          <t>e.Keith@gmail.com</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>G.David@gmail.com</t>
+          <t>g.David@gmail.com</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>G.Don@gmail.com</t>
+          <t>g.Don@gmail.com</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>H.Ashir@gmail.com</t>
+          <t>h.Ashir@gmail.com</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -792,7 +792,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>H.Fardowsa@gmail.com</t>
+          <t>h.Fardowsa@gmail.com</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -820,7 +820,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>I.Ruweida@gmail.com</t>
+          <t>i.Ruweida@gmail.com</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>J.Myles@gmail.com</t>
+          <t>j.Myles@gmail.com</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>K.Ann@gmail.com</t>
+          <t>k.Ann@gmail.com</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -904,7 +904,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>K.Sharon@gmail.com</t>
+          <t>k.Sharon@gmail.com</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -932,7 +932,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>K.Neema@gmail.com</t>
+          <t>k.Neema@gmail.com</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -960,7 +960,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>K.Samuel@gmail.com</t>
+          <t>k.Samuel@gmail.com</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -988,7 +988,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>K.Shannon@gmail.com</t>
+          <t>k.Shannon@gmail.com</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>K.Peter@gmail.com</t>
+          <t>k.Peter@gmail.com</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>K.Victor@gmail.com</t>
+          <t>k.Victor@gmail.com</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>K.Ian@gmail.com</t>
+          <t>k.Ian@gmail.com</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1100,7 +1100,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>K.Eric@gmail.com</t>
+          <t>k.Eric@gmail.com</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1128,7 +1128,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>K.Kevin@gmail.com</t>
+          <t>k.Kevin@gmail.com</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>K.Alex@gmail.com</t>
+          <t>k.Alex@gmail.com</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>M.Kelvin@gmail.com</t>
+          <t>m.Kelvin@gmail.com</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>M.Zivai@gmail.com</t>
+          <t>m.Zivai@gmail.com</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>M.Ally@gmail.com</t>
+          <t>m.Ally@gmail.com</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>M.David@gmail.com</t>
+          <t>m.David@gmail.com</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>M.Kelvin@gmail.com</t>
+          <t>m.Kelvin@gmail.com</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>M.Victor@gmail.com</t>
+          <t>m.Victor@gmail.com</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1352,7 +1352,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>M.Natasha@gmail.com</t>
+          <t>m.Natasha@gmail.com</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>M.Grace@gmail.com</t>
+          <t>m.Grace@gmail.com</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>M.Mark@gmail.com</t>
+          <t>m.Mark@gmail.com</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>M.Ruby@gmail.com</t>
+          <t>m.Ruby@gmail.com</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>M.Franklin@gmail.com</t>
+          <t>m.Franklin@gmail.com</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>M.Eric@gmail.com</t>
+          <t>m.Eric@gmail.com</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1520,7 +1520,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>M.Patience@gmail.com</t>
+          <t>m.Patience@gmail.com</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>M.George@gmail.com</t>
+          <t>m.George@gmail.com</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>N.Andrew@gmail.com</t>
+          <t>n.Andrew@gmail.com</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>N.Monicah@gmail.com</t>
+          <t>n.Monicah@gmail.com</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>N.Yvonne@gmail.com</t>
+          <t>n.Yvonne@gmail.com</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>N.Sarah@gmail.com</t>
+          <t>n.Sarah@gmail.com</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>N.Ian@gmail.com</t>
+          <t>n.Ian@gmail.com</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>N.Alvin@gmail.com</t>
+          <t>n.Alvin@gmail.com</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>N.Michael@gmail.com</t>
+          <t>n.Michael@gmail.com</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>N.Elizabeth@gmail.com</t>
+          <t>n.Elizabeth@gmail.com</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>N.Andrew@gmail.com</t>
+          <t>n.Andrew@gmail.com</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>N.Erica@gmail.com</t>
+          <t>n.Erica@gmail.com</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>N.Maureen@gmail.com</t>
+          <t>n.Maureen@gmail.com</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>O.Steven@gmail.com</t>
+          <t>o.Steven@gmail.com</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -1912,7 +1912,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>O.Brenda@gmail.com</t>
+          <t>o.Brenda@gmail.com</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -1940,7 +1940,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>O.Mwenzangu@gmail.com</t>
+          <t>o.Mwenzangu@gmail.com</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>O.Caleb@gmail.com</t>
+          <t>o.Caleb@gmail.com</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>O.Charis@gmail.com</t>
+          <t>o.Charis@gmail.com</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2024,7 +2024,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>O.Nicole@gmail.com</t>
+          <t>o.Nicole@gmail.com</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>P.Jay@gmail.com</t>
+          <t>p.Jay@gmail.com</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2080,7 +2080,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>T.Martin@gmail.com</t>
+          <t>t.Martin@gmail.com</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2108,7 +2108,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>T.Bramwel@gmail.com</t>
+          <t>t.Bramwel@gmail.com</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>W.Joy@gmail.com</t>
+          <t>w.Joy@gmail.com</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2164,7 +2164,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>W.Rosemary@gmail.com</t>
+          <t>w.Rosemary@gmail.com</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2192,7 +2192,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>W.Louis@gmail.com</t>
+          <t>w.Louis@gmail.com</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2220,7 +2220,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>W.Monika@gmail.com</t>
+          <t>w.Monika@gmail.com</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>W.Trevor@gmail.com</t>
+          <t>w.Trevor@gmail.com</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">

</xml_diff>

<commit_message>
Fixed some code error
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>aAdrian@gmail.com</t>
+          <t>apaul@gmail.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>aShanelle@gmail.com</t>
+          <t>aanyango@gmail.com</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>aJude@gmail.com</t>
+          <t>aocomil@gmail.com</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -564,7 +564,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>aKyla@gmail.com</t>
+          <t>aneema@gmail.com</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -590,7 +590,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>aAnthony@gmail.com</t>
+          <t>aikobwa@gmail.com</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>bMoses@gmail.com</t>
+          <t>bkasuni@gmail.com</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -642,7 +642,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>dKalid@gmail.com</t>
+          <t>dgeleta@gmail.com</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>eKeith@gmail.com</t>
+          <t>elokwei@gmail.com</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>gDavid@gmail.com</t>
+          <t>gotieno@gmail.com</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -720,7 +720,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>gDon@gmail.com</t>
+          <t>gthigiti@gmail.com</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>hAshir@gmail.com</t>
+          <t>hali@gmail.com</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -772,7 +772,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>hFardowsa@gmail.com</t>
+          <t>habduhakim@gmail.com</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>iRuweida@gmail.com</t>
+          <t>iali@gmail.com</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>jMyles@gmail.com</t>
+          <t>jadebayo@gmail.com</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -850,7 +850,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>kAnn@gmail.com</t>
+          <t>kmumbi@gmail.com</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>kSharon@gmail.com</t>
+          <t>kwanjiru@gmail.com</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -902,7 +902,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>kNeema@gmail.com</t>
+          <t>kmuthoni@gmail.com</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>kSamuel@gmail.com</t>
+          <t>kndungu@gmail.com</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -954,7 +954,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>kShannon@gmail.com</t>
+          <t>kkendi@gmail.com</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -980,7 +980,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>kPeter@gmail.com</t>
+          <t>kkibet@gmail.com</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>kVictor@gmail.com</t>
+          <t>kmfana@gmail.com</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1032,7 +1032,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>kIan@gmail.com</t>
+          <t>kmuteithia@gmail.com</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>kEric@gmail.com</t>
+          <t>kmuriithi@gmail.com</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>kKevin@gmail.com</t>
+          <t>kkimutai@gmail.com</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1110,7 +1110,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>kAlex@gmail.com</t>
+          <t>kwafula@gmail.com</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>mKelvin@gmail.com</t>
+          <t>mkipngeno@gmail.com</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>mZivai@gmail.com</t>
+          <t>mdavid@gmail.com</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>mAlly@gmail.com</t>
+          <t>mmahamud@gmail.com</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1214,7 +1214,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>mDavid@gmail.com</t>
+          <t>mnyamongo@gmail.com</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>mKelvin@gmail.com</t>
+          <t>mkarani@gmail.com</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>mVictor@gmail.com</t>
+          <t>mmwaura@gmail.com</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>mNatasha@gmail.com</t>
+          <t>mwaithira@gmail.com</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>mGrace@gmail.com</t>
+          <t>mkanini@gmail.com</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>mMark@gmail.com</t>
+          <t>mgichuhi@gmail.com</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>mRuby@gmail.com</t>
+          <t>mmbete@gmail.com</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>mFranklin@gmail.com</t>
+          <t>mkaranja@gmail.com</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>mEric@gmail.com</t>
+          <t>mkiamba@gmail.com</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>mPatience@gmail.com</t>
+          <t>mkamanthe@gmail.com</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>mGeorge@gmail.com</t>
+          <t>mjosiah@gmail.com</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>nAndrew@gmail.com</t>
+          <t>nkasaine@gmail.com</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>nMonicah@gmail.com</t>
+          <t>nmonicah@gmail.com</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>nYvonne@gmail.com</t>
+          <t>nnyambura@gmail.com</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1578,7 +1578,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>nSarah@gmail.com</t>
+          <t>nwangari@gmail.com</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>nIan@gmail.com</t>
+          <t>nmutuge@gmail.com</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>nAlvin@gmail.com</t>
+          <t>nkipkurui@gmail.com</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>nMichael@gmail.com</t>
+          <t>nmacharia@gmail.com</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>nElizabeth@gmail.com</t>
+          <t>nnjoki@gmail.com</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>nAndrew@gmail.com</t>
+          <t>nkiarie@gmail.com</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1734,7 +1734,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>nErica@gmail.com</t>
+          <t>nerica@gmail.com</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>nMaureen@gmail.com</t>
+          <t>nmutete@gmail.com</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>oSteven@gmail.com</t>
+          <t>ojona@gmail.com</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -1812,7 +1812,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>oBrenda@gmail.com</t>
+          <t>oanyango@gmail.com</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>oMwenzangu@gmail.com</t>
+          <t>ofaraja@gmail.com</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>oCaleb@gmail.com</t>
+          <t>omagare@gmail.com</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -1890,7 +1890,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>oCharis@gmail.com</t>
+          <t>ong'wono@gmail.com</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>oNicole@gmail.com</t>
+          <t>oowens@gmail.com</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>pJay@gmail.com</t>
+          <t>phirji@gmail.com</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>tMartin@gmail.com</t>
+          <t>tmartin@gmail.com</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>tBramwel@gmail.com</t>
+          <t>tkipchirchir@gmail.com</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2020,7 +2020,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>wJoy@gmail.com</t>
+          <t>wmuthoni@gmail.com</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>wRosemary@gmail.com</t>
+          <t>wnjeri@gmail.com</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>wLouis@gmail.com</t>
+          <t>wmbugua@gmail.com</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>wMonika@gmail.com</t>
+          <t>wng'endo@gmail.com</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>wTrevor@gmail.com</t>
+          <t>wkariuki@gmail.com</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">

</xml_diff>